<commit_message>
photos and Yanick updates
</commit_message>
<xml_diff>
--- a/forms/app/pev_femme.xlsx
+++ b/forms/app/pev_femme.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="834" uniqueCount="569">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="833" uniqueCount="568">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -258,9 +258,6 @@
   </si>
   <si>
     <t xml:space="preserve">_case_date_vat1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">if(instance('contact-summary')/context/imm_date vat1!='',date(instance('contact-summary')/context/imm_date vat1),'')</t>
   </si>
   <si>
     <t xml:space="preserve">_case_date_vat2</t>
@@ -3602,12 +3599,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
-    <numFmt numFmtId="166" formatCode="General"/>
-    <numFmt numFmtId="167" formatCode="0"/>
-    <numFmt numFmtId="168" formatCode="d\-mmm"/>
+    <numFmt numFmtId="166" formatCode="0"/>
+    <numFmt numFmtId="167" formatCode="d\-mmm"/>
   </numFmts>
   <fonts count="18">
     <font>
@@ -4009,7 +4005,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4097,7 +4093,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4197,7 +4193,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="17" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="17" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -9142,11 +9138,11 @@
   <dimension ref="A1:Z1011"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="D90" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="K20" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A90" activeCellId="0" sqref="A90"/>
-      <selection pane="bottomRight" activeCell="J97" activeCellId="0" sqref="J97"/>
+      <selection pane="topRight" activeCell="K1" activeCellId="0" sqref="K1"/>
+      <selection pane="bottomLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
+      <selection pane="bottomRight" activeCell="P32" activeCellId="0" sqref="P32:P36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.0078125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
@@ -9772,14 +9768,12 @@
       <c r="J32" s="4"/>
       <c r="K32" s="4"/>
       <c r="L32" s="4"/>
-      <c r="M32" s="4" t="s">
-        <v>76</v>
-      </c>
+      <c r="M32" s="4"/>
       <c r="N32" s="4"/>
       <c r="O32" s="4"/>
       <c r="P32" s="15" t="str">
-        <f aca="false">_xlfn.CONCAT("if(coalesce(instance('contact-summary')/context/imm_",C23,",'')!='',date(instance('contact-summary')/context/imm_",C23,"),'')")</f>
-        <v>if(coalesce(instance('contact-summary')/context/imm_,'')!='',date(instance('contact-summary')/context/imm_),'')</v>
+        <f aca="false">_xlfn.CONCAT("if(coalesce(instance('contact-summary')/context/imm_",C32,",'')!='',date(instance('contact-summary')/context/imm_",C32,"),'')")</f>
+        <v>if(coalesce(instance('contact-summary')/context/imm_date_vat1,'')!='',date(instance('contact-summary')/context/imm_date_vat1),'')</v>
       </c>
       <c r="Q32" s="4"/>
       <c r="R32" s="4"/>
@@ -9797,7 +9791,7 @@
         <v>58</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>64</v>
@@ -9815,8 +9809,8 @@
       <c r="N33" s="4"/>
       <c r="O33" s="4"/>
       <c r="P33" s="15" t="str">
-        <f aca="false">_xlfn.CONCAT("if(coalesce(instance('contact-summary')/context/imm_",C24,",'')!='',date(instance('contact-summary')/context/imm_",C24,"),'')")</f>
-        <v>if(coalesce(instance('contact-summary')/context/imm_,'')!='',date(instance('contact-summary')/context/imm_),'')</v>
+        <f aca="false">_xlfn.CONCAT("if(coalesce(instance('contact-summary')/context/imm_",C33,",'')!='',date(instance('contact-summary')/context/imm_",C33,"),'')")</f>
+        <v>if(coalesce(instance('contact-summary')/context/imm_date_vat2,'')!='',date(instance('contact-summary')/context/imm_date_vat2),'')</v>
       </c>
       <c r="Q33" s="4"/>
       <c r="R33" s="4"/>
@@ -9834,7 +9828,7 @@
         <v>58</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>66</v>
@@ -9852,8 +9846,8 @@
       <c r="N34" s="4"/>
       <c r="O34" s="4"/>
       <c r="P34" s="15" t="str">
-        <f aca="false">_xlfn.CONCAT("if(coalesce(instance('contact-summary')/context/imm_",C25,",'')!='',date(instance('contact-summary')/context/imm_",C25,"),'')")</f>
-        <v>if(coalesce(instance('contact-summary')/context/imm_,'')!='',date(instance('contact-summary')/context/imm_),'')</v>
+        <f aca="false">_xlfn.CONCAT("if(coalesce(instance('contact-summary')/context/imm_",C34,",'')!='',date(instance('contact-summary')/context/imm_",C34,"),'')")</f>
+        <v>if(coalesce(instance('contact-summary')/context/imm_date_vat3,'')!='',date(instance('contact-summary')/context/imm_date_vat3),'')</v>
       </c>
       <c r="Q34" s="4"/>
       <c r="R34" s="4"/>
@@ -9871,7 +9865,7 @@
         <v>58</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>68</v>
@@ -9889,8 +9883,8 @@
       <c r="N35" s="4"/>
       <c r="O35" s="4"/>
       <c r="P35" s="15" t="str">
-        <f aca="false">_xlfn.CONCAT("if(coalesce(instance('contact-summary')/context/imm_",C26,",'')!='',date(instance('contact-summary')/context/imm_",C26,"),'')")</f>
-        <v>if(coalesce(instance('contact-summary')/context/imm_,'')!='',date(instance('contact-summary')/context/imm_),'')</v>
+        <f aca="false">_xlfn.CONCAT("if(coalesce(instance('contact-summary')/context/imm_",C35,",'')!='',date(instance('contact-summary')/context/imm_",C35,"),'')")</f>
+        <v>if(coalesce(instance('contact-summary')/context/imm_date_vat4,'')!='',date(instance('contact-summary')/context/imm_date_vat4),'')</v>
       </c>
       <c r="Q35" s="4"/>
       <c r="R35" s="4"/>
@@ -9908,7 +9902,7 @@
         <v>58</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>70</v>
@@ -9926,8 +9920,8 @@
       <c r="N36" s="4"/>
       <c r="O36" s="4"/>
       <c r="P36" s="15" t="str">
-        <f aca="false">_xlfn.CONCAT("if(coalesce(instance('contact-summary')/context/imm_",C27,",'')!='',date(instance('contact-summary')/context/imm_",C27,"),'')")</f>
-        <v>if(coalesce(instance('contact-summary')/context/imm_,'')!='',date(instance('contact-summary')/context/imm_),'')</v>
+        <f aca="false">_xlfn.CONCAT("if(coalesce(instance('contact-summary')/context/imm_",C36,",'')!='',date(instance('contact-summary')/context/imm_",C36,"),'')")</f>
+        <v>if(coalesce(instance('contact-summary')/context/imm_date_vat5,'')!='',date(instance('contact-summary')/context/imm_date_vat5),'')</v>
       </c>
       <c r="Q36" s="4"/>
       <c r="R36" s="4"/>
@@ -10200,10 +10194,10 @@
         <v>26</v>
       </c>
       <c r="B50" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C50" s="17" t="s">
         <v>81</v>
-      </c>
-      <c r="C50" s="17" t="s">
-        <v>82</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>29</v>
@@ -10212,13 +10206,13 @@
     </row>
     <row r="51" s="8" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="C51" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>85</v>
       </c>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
@@ -10235,7 +10229,7 @@
       <c r="N51" s="1"/>
       <c r="O51" s="1"/>
       <c r="P51" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Q51" s="1"/>
       <c r="R51" s="1"/>
@@ -10257,11 +10251,11 @@
         <v>58</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C53" s="12"/>
       <c r="P53" s="13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="54" s="8" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10269,11 +10263,11 @@
         <v>58</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C54" s="12"/>
       <c r="P54" s="13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="55" s="8" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10281,11 +10275,11 @@
         <v>58</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C55" s="12"/>
       <c r="P55" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="56" s="8" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10293,11 +10287,11 @@
         <v>58</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C56" s="12"/>
       <c r="P56" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="57" s="8" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10305,11 +10299,11 @@
         <v>58</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C57" s="12"/>
       <c r="P57" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="58" s="8" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10321,11 +10315,11 @@
         <v>58</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C64" s="12"/>
       <c r="P64" s="13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="65" s="8" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10333,11 +10327,11 @@
         <v>58</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C65" s="12"/>
       <c r="P65" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="66" s="8" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10345,11 +10339,11 @@
         <v>58</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C66" s="12"/>
       <c r="P66" s="13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="67" s="8" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10357,11 +10351,11 @@
         <v>58</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C67" s="12"/>
       <c r="P67" s="13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="68" s="8" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10369,11 +10363,11 @@
         <v>58</v>
       </c>
       <c r="B68" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C68" s="12"/>
       <c r="P68" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="69" s="8" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10381,19 +10375,19 @@
         <v>45</v>
       </c>
       <c r="B69" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="C69" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="C69" s="8" t="s">
+      <c r="H69" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="H69" s="8" t="s">
+      <c r="I69" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="I69" s="8" t="s">
+      <c r="J69" s="8" t="s">
         <v>110</v>
-      </c>
-      <c r="J69" s="8" t="s">
-        <v>111</v>
       </c>
       <c r="L69" s="8" t="n">
         <v>1</v>
@@ -10405,19 +10399,19 @@
         <v>45</v>
       </c>
       <c r="B70" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C70" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="C70" s="8" t="s">
+      <c r="H70" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="H70" s="8" t="s">
+      <c r="I70" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="J70" s="8" t="s">
         <v>114</v>
-      </c>
-      <c r="I70" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="J70" s="8" t="s">
-        <v>115</v>
       </c>
       <c r="L70" s="8" t="n">
         <v>1</v>
@@ -10429,19 +10423,19 @@
         <v>45</v>
       </c>
       <c r="B71" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="C71" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="C71" s="8" t="s">
+      <c r="H71" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="H71" s="8" t="s">
+      <c r="I71" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="J71" s="8" t="s">
         <v>118</v>
-      </c>
-      <c r="I71" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="J71" s="8" t="s">
-        <v>119</v>
       </c>
       <c r="L71" s="8" t="n">
         <v>1</v>
@@ -10453,19 +10447,19 @@
         <v>45</v>
       </c>
       <c r="B72" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="C72" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="C72" s="8" t="s">
+      <c r="H72" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="H72" s="8" t="s">
+      <c r="I72" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="J72" s="8" t="s">
         <v>122</v>
-      </c>
-      <c r="I72" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="J72" s="8" t="s">
-        <v>123</v>
       </c>
       <c r="L72" s="8" t="n">
         <v>1</v>
@@ -10477,19 +10471,19 @@
         <v>45</v>
       </c>
       <c r="B73" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="C73" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="C73" s="8" t="s">
+      <c r="H73" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="H73" s="8" t="s">
+      <c r="I73" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="J73" s="8" t="s">
         <v>126</v>
-      </c>
-      <c r="I73" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="J73" s="8" t="s">
-        <v>127</v>
       </c>
       <c r="L73" s="8" t="n">
         <v>1</v>
@@ -10501,11 +10495,11 @@
         <v>58</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C74" s="12"/>
       <c r="P74" s="13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10513,10 +10507,10 @@
         <v>58</v>
       </c>
       <c r="B75" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="P75" s="13" t="s">
         <v>130</v>
-      </c>
-      <c r="P75" s="13" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10524,10 +10518,10 @@
         <v>58</v>
       </c>
       <c r="B76" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="P76" s="13" t="s">
         <v>132</v>
-      </c>
-      <c r="P76" s="13" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10535,10 +10529,10 @@
         <v>58</v>
       </c>
       <c r="B77" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="P77" s="13" t="s">
         <v>134</v>
-      </c>
-      <c r="P77" s="13" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -10547,26 +10541,26 @@
         <v>58</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C79" s="18"/>
       <c r="J79" s="18"/>
       <c r="P79" s="13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B80" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B80" s="1" t="s">
+      <c r="C80" s="18" t="s">
         <v>139</v>
       </c>
-      <c r="C80" s="18" t="s">
+      <c r="J80" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="J80" s="1" t="s">
-        <v>141</v>
       </c>
       <c r="L80" s="1" t="n">
         <v>1</v>
@@ -10578,13 +10572,13 @@
         <v>22</v>
       </c>
       <c r="B81" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C81" s="18" t="s">
         <v>142</v>
       </c>
-      <c r="C81" s="18" t="s">
+      <c r="J81" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="J81" s="1" t="s">
-        <v>144</v>
       </c>
       <c r="P81" s="13"/>
     </row>
@@ -10593,25 +10587,25 @@
         <v>58</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C82" s="18"/>
       <c r="P82" s="19" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B83" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C83" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="C83" s="18" t="s">
+      <c r="J83" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="J83" s="1" t="s">
-        <v>149</v>
       </c>
       <c r="L83" s="1" t="n">
         <v>1</v>
@@ -10623,13 +10617,13 @@
         <v>22</v>
       </c>
       <c r="B84" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C84" s="18" t="s">
         <v>150</v>
       </c>
-      <c r="C84" s="18" t="s">
+      <c r="J84" s="1" t="s">
         <v>151</v>
-      </c>
-      <c r="J84" s="1" t="s">
-        <v>152</v>
       </c>
       <c r="P84" s="13"/>
     </row>
@@ -10638,25 +10632,25 @@
         <v>58</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C85" s="18"/>
       <c r="P85" s="19" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B86" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C86" s="18" t="s">
         <v>155</v>
       </c>
-      <c r="C86" s="18" t="s">
+      <c r="J86" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="J86" s="1" t="s">
-        <v>157</v>
       </c>
       <c r="L86" s="1" t="n">
         <v>1</v>
@@ -10668,13 +10662,13 @@
         <v>22</v>
       </c>
       <c r="B87" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C87" s="18" t="s">
         <v>158</v>
       </c>
-      <c r="C87" s="18" t="s">
+      <c r="J87" s="1" t="s">
         <v>159</v>
-      </c>
-      <c r="J87" s="1" t="s">
-        <v>160</v>
       </c>
       <c r="P87" s="13"/>
     </row>
@@ -10683,25 +10677,25 @@
         <v>58</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C88" s="18"/>
       <c r="P88" s="19" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B89" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C89" s="18" t="s">
         <v>163</v>
       </c>
-      <c r="C89" s="18" t="s">
+      <c r="J89" s="1" t="s">
         <v>164</v>
-      </c>
-      <c r="J89" s="1" t="s">
-        <v>165</v>
       </c>
       <c r="L89" s="1" t="n">
         <v>1</v>
@@ -10713,13 +10707,13 @@
         <v>22</v>
       </c>
       <c r="B90" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C90" s="18" t="s">
         <v>166</v>
       </c>
-      <c r="C90" s="18" t="s">
+      <c r="J90" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="J90" s="1" t="s">
-        <v>168</v>
       </c>
       <c r="P90" s="13"/>
     </row>
@@ -10728,25 +10722,25 @@
         <v>58</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C91" s="18"/>
       <c r="P91" s="13" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B92" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C92" s="18" t="s">
         <v>171</v>
       </c>
-      <c r="C92" s="18" t="s">
+      <c r="J92" s="1" t="s">
         <v>172</v>
-      </c>
-      <c r="J92" s="1" t="s">
-        <v>173</v>
       </c>
       <c r="L92" s="1" t="n">
         <v>1</v>
@@ -10758,13 +10752,13 @@
         <v>22</v>
       </c>
       <c r="B93" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C93" s="18" t="s">
         <v>174</v>
       </c>
-      <c r="C93" s="18" t="s">
+      <c r="J93" s="1" t="s">
         <v>175</v>
-      </c>
-      <c r="J93" s="1" t="s">
-        <v>176</v>
       </c>
       <c r="P93" s="13"/>
     </row>
@@ -10773,13 +10767,13 @@
         <v>22</v>
       </c>
       <c r="B95" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C95" s="18" t="s">
         <v>177</v>
       </c>
-      <c r="C95" s="18" t="s">
+      <c r="J95" s="19" t="s">
         <v>178</v>
-      </c>
-      <c r="J95" s="19" t="s">
-        <v>179</v>
       </c>
       <c r="P95" s="13"/>
     </row>
@@ -10788,13 +10782,13 @@
         <v>22</v>
       </c>
       <c r="B96" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C96" s="20" t="s">
         <v>180</v>
       </c>
-      <c r="C96" s="20" t="s">
+      <c r="J96" s="1" t="s">
         <v>181</v>
-      </c>
-      <c r="J96" s="1" t="s">
-        <v>182</v>
       </c>
       <c r="P96" s="13"/>
     </row>
@@ -10803,13 +10797,13 @@
         <v>22</v>
       </c>
       <c r="B97" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C97" s="18" t="s">
         <v>183</v>
       </c>
-      <c r="C97" s="18" t="s">
+      <c r="J97" s="1" t="s">
         <v>184</v>
-      </c>
-      <c r="J97" s="1" t="s">
-        <v>185</v>
       </c>
       <c r="P97" s="13"/>
     </row>
@@ -10818,7 +10812,7 @@
         <v>57</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C98" s="17"/>
       <c r="P98" s="13"/>
@@ -10828,10 +10822,10 @@
         <v>26</v>
       </c>
       <c r="B99" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C99" s="18" t="s">
         <v>186</v>
-      </c>
-      <c r="C99" s="18" t="s">
-        <v>187</v>
       </c>
       <c r="G99" s="1" t="s">
         <v>29</v>
@@ -10843,13 +10837,13 @@
         <v>22</v>
       </c>
       <c r="B100" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C100" s="18" t="s">
         <v>188</v>
       </c>
-      <c r="C100" s="18" t="s">
+      <c r="J100" s="1" t="s">
         <v>189</v>
-      </c>
-      <c r="J100" s="1" t="s">
-        <v>190</v>
       </c>
       <c r="P100" s="13"/>
     </row>
@@ -10858,13 +10852,13 @@
         <v>22</v>
       </c>
       <c r="B101" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C101" s="18" t="s">
         <v>191</v>
       </c>
-      <c r="C101" s="18" t="s">
+      <c r="J101" s="1" t="s">
         <v>192</v>
-      </c>
-      <c r="J101" s="1" t="s">
-        <v>193</v>
       </c>
       <c r="P101" s="13"/>
     </row>
@@ -10873,13 +10867,13 @@
         <v>22</v>
       </c>
       <c r="B102" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C102" s="18" t="s">
         <v>194</v>
       </c>
-      <c r="C102" s="18" t="s">
+      <c r="J102" s="1" t="s">
         <v>195</v>
-      </c>
-      <c r="J102" s="1" t="s">
-        <v>196</v>
       </c>
       <c r="P102" s="13"/>
     </row>
@@ -10888,13 +10882,13 @@
         <v>22</v>
       </c>
       <c r="B103" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C103" s="18" t="s">
         <v>197</v>
       </c>
-      <c r="C103" s="18" t="s">
+      <c r="J103" s="1" t="s">
         <v>198</v>
-      </c>
-      <c r="J103" s="1" t="s">
-        <v>199</v>
       </c>
       <c r="P103" s="13"/>
     </row>
@@ -10903,13 +10897,13 @@
         <v>22</v>
       </c>
       <c r="B104" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C104" s="18" t="s">
         <v>200</v>
       </c>
-      <c r="C104" s="18" t="s">
+      <c r="J104" s="1" t="s">
         <v>201</v>
-      </c>
-      <c r="J104" s="1" t="s">
-        <v>202</v>
       </c>
       <c r="P104" s="13"/>
     </row>
@@ -10918,7 +10912,7 @@
         <v>57</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C105" s="18"/>
       <c r="P105" s="13"/>
@@ -35988,46 +35982,46 @@
   </conditionalFormatting>
   <conditionalFormatting sqref="K441 W427:Z440 K596:Z597 B596:I597 A604:F604 B605:F606 G604:G609 A607:F609 A610:G612 A441:I441 A457:C457 B601:C601 M603:Z603 M607:Z611 L603:L612 W442:Z454 L427:V454">
     <cfRule type="expression" priority="104" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="102">
-      <formula>OR($A371="date", $A371="datetime")</formula>
+      <formula>OR($A357="date", $A357="datetime")</formula>
     </cfRule>
     <cfRule type="expression" priority="105" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="103">
-      <formula>OR($A371="calculate", $A371="calculate_here")</formula>
+      <formula>OR($A357="calculate", $A357="calculate_here")</formula>
     </cfRule>
     <cfRule type="expression" priority="106" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="104">
-      <formula>$A371="note"</formula>
+      <formula>$A357="note"</formula>
     </cfRule>
     <cfRule type="expression" priority="107" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="105">
-      <formula>$A371="barcode"</formula>
+      <formula>$A357="barcode"</formula>
     </cfRule>
     <cfRule type="expression" priority="108" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="106">
-      <formula>OR($A371="geopoint", $A371="geoshape", $A371="geotrace")</formula>
+      <formula>OR($A357="geopoint", $A357="geoshape", $A357="geotrace")</formula>
     </cfRule>
     <cfRule type="expression" priority="109" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="107">
-      <formula>OR($A371="username", $A371="phonenumber", $A371="start", $A371="end", $A371="deviceid", $A371="subscriberid", $A371="simserial", $A371="caseid")</formula>
+      <formula>OR($A357="username", $A357="phonenumber", $A357="start", $A357="end", $A357="deviceid", $A357="subscriberid", $A357="simserial", $A357="caseid")</formula>
     </cfRule>
     <cfRule type="expression" priority="110" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="108">
-      <formula>OR(AND(LEFT($A371, 16)="select_multiple ", LEN($A371)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A371, 17)))), AND(LEFT($A371, 11)="select_one ", LEN($A371)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A371, 12)))))</formula>
+      <formula>OR(AND(LEFT($A357, 16)="select_multiple ", LEN($A357)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A357, 17)))), AND(LEFT($A357, 11)="select_one ", LEN($A357)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A357, 12)))))</formula>
     </cfRule>
     <cfRule type="expression" priority="111" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="109">
-      <formula>$A371="decimal"</formula>
+      <formula>$A357="decimal"</formula>
     </cfRule>
     <cfRule type="expression" priority="112" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="110">
-      <formula>$A371="integer"</formula>
+      <formula>$A357="integer"</formula>
     </cfRule>
     <cfRule type="expression" priority="113" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="111">
-      <formula>$A371="text"</formula>
+      <formula>$A357="text"</formula>
     </cfRule>
     <cfRule type="expression" priority="114" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="112">
-      <formula>$A371="end repeat"</formula>
+      <formula>$A357="end repeat"</formula>
     </cfRule>
     <cfRule type="expression" priority="115" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="113">
-      <formula>$A371="begin repeat"</formula>
+      <formula>$A357="begin repeat"</formula>
     </cfRule>
     <cfRule type="expression" priority="116" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="114">
-      <formula>$A371="end group"</formula>
+      <formula>$A357="end group"</formula>
     </cfRule>
     <cfRule type="expression" priority="117" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="115">
-      <formula>$A371="begin group"</formula>
+      <formula>$A357="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B588:B592 B596 B607:B611 B598:B602 B463:B464 B416:B424 B466:B478 B426:B440 B442:B458 B480:B540 B566:B567 B578:B586 B257:B280 B542:B548 B550:B564 B282:B322 B325:B413 B570:B576 B151:B248 B613:B617 B251:B255">
@@ -36285,46 +36279,46 @@
   </conditionalFormatting>
   <conditionalFormatting sqref="A605:A606 M604:Z604">
     <cfRule type="expression" priority="179" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="177">
-      <formula>OR($A600="date", $A600="datetime")</formula>
+      <formula>OR($A599="date", $A599="datetime")</formula>
     </cfRule>
     <cfRule type="expression" priority="180" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="178">
-      <formula>OR($A600="calculate", $A600="calculate_here")</formula>
+      <formula>OR($A599="calculate", $A599="calculate_here")</formula>
     </cfRule>
     <cfRule type="expression" priority="181" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="179">
-      <formula>$A600="note"</formula>
+      <formula>$A599="note"</formula>
     </cfRule>
     <cfRule type="expression" priority="182" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="180">
-      <formula>$A600="barcode"</formula>
+      <formula>$A599="barcode"</formula>
     </cfRule>
     <cfRule type="expression" priority="183" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="181">
-      <formula>OR($A600="geopoint", $A600="geoshape", $A600="geotrace")</formula>
+      <formula>OR($A599="geopoint", $A599="geoshape", $A599="geotrace")</formula>
     </cfRule>
     <cfRule type="expression" priority="184" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="182">
-      <formula>OR($A600="username", $A600="phonenumber", $A600="start", $A600="end", $A600="deviceid", $A600="subscriberid", $A600="simserial", $A600="caseid")</formula>
+      <formula>OR($A599="username", $A599="phonenumber", $A599="start", $A599="end", $A599="deviceid", $A599="subscriberid", $A599="simserial", $A599="caseid")</formula>
     </cfRule>
     <cfRule type="expression" priority="185" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="183">
-      <formula>OR(AND(LEFT($A600, 16)="select_multiple ", LEN($A600)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A600, 17)))), AND(LEFT($A600, 11)="select_one ", LEN($A600)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A600, 12)))))</formula>
+      <formula>OR(AND(LEFT($A599, 16)="select_multiple ", LEN($A599)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A599, 17)))), AND(LEFT($A599, 11)="select_one ", LEN($A599)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A599, 12)))))</formula>
     </cfRule>
     <cfRule type="expression" priority="186" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="184">
-      <formula>$A600="decimal"</formula>
+      <formula>$A599="decimal"</formula>
     </cfRule>
     <cfRule type="expression" priority="187" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="185">
-      <formula>$A600="integer"</formula>
+      <formula>$A599="integer"</formula>
     </cfRule>
     <cfRule type="expression" priority="188" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="186">
-      <formula>$A600="text"</formula>
+      <formula>$A599="text"</formula>
     </cfRule>
     <cfRule type="expression" priority="189" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="187">
-      <formula>$A600="end repeat"</formula>
+      <formula>$A599="end repeat"</formula>
     </cfRule>
     <cfRule type="expression" priority="190" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="188">
-      <formula>$A600="begin repeat"</formula>
+      <formula>$A599="begin repeat"</formula>
     </cfRule>
     <cfRule type="expression" priority="191" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="189">
-      <formula>$A600="end group"</formula>
+      <formula>$A599="end group"</formula>
     </cfRule>
     <cfRule type="expression" priority="192" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="190">
-      <formula>$A600="begin group"</formula>
+      <formula>$A599="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B603:B604">
@@ -37231,46 +37225,46 @@
   </conditionalFormatting>
   <conditionalFormatting sqref="L146:Z149 A147:F149">
     <cfRule type="expression" priority="411" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="409">
-      <formula>OR($A142="date", $A142="datetime")</formula>
+      <formula>OR($A141="date", $A141="datetime")</formula>
     </cfRule>
     <cfRule type="expression" priority="412" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="410">
-      <formula>OR($A142="calculate", $A142="calculate_here")</formula>
+      <formula>OR($A141="calculate", $A141="calculate_here")</formula>
     </cfRule>
     <cfRule type="expression" priority="413" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="411">
-      <formula>$A142="note"</formula>
+      <formula>$A141="note"</formula>
     </cfRule>
     <cfRule type="expression" priority="414" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="412">
-      <formula>$A142="barcode"</formula>
+      <formula>$A141="barcode"</formula>
     </cfRule>
     <cfRule type="expression" priority="415" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="413">
-      <formula>OR($A142="geopoint", $A142="geoshape", $A142="geotrace")</formula>
+      <formula>OR($A141="geopoint", $A141="geoshape", $A141="geotrace")</formula>
     </cfRule>
     <cfRule type="expression" priority="416" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="414">
-      <formula>OR($A142="username", $A142="phonenumber", $A142="start", $A142="end", $A142="deviceid", $A142="subscriberid", $A142="simserial", $A142="caseid")</formula>
+      <formula>OR($A141="username", $A141="phonenumber", $A141="start", $A141="end", $A141="deviceid", $A141="subscriberid", $A141="simserial", $A141="caseid")</formula>
     </cfRule>
     <cfRule type="expression" priority="417" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="415">
-      <formula>OR(AND(LEFT($A142, 16)="select_multiple ", LEN($A142)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A142, 17)))), AND(LEFT($A142, 11)="select_one ", LEN($A142)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A142, 12)))))</formula>
+      <formula>OR(AND(LEFT($A141, 16)="select_multiple ", LEN($A141)&gt;16, NOT(ISNUMBER(SEARCH(" ", $A141, 17)))), AND(LEFT($A141, 11)="select_one ", LEN($A141)&gt;11, NOT(ISNUMBER(SEARCH(" ", $A141, 12)))))</formula>
     </cfRule>
     <cfRule type="expression" priority="418" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="416">
-      <formula>$A142="decimal"</formula>
+      <formula>$A141="decimal"</formula>
     </cfRule>
     <cfRule type="expression" priority="419" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="417">
-      <formula>$A142="integer"</formula>
+      <formula>$A141="integer"</formula>
     </cfRule>
     <cfRule type="expression" priority="420" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="418">
-      <formula>$A142="text"</formula>
+      <formula>$A141="text"</formula>
     </cfRule>
     <cfRule type="expression" priority="421" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="419">
-      <formula>$A142="end repeat"</formula>
+      <formula>$A141="end repeat"</formula>
     </cfRule>
     <cfRule type="expression" priority="422" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="420">
-      <formula>$A142="begin repeat"</formula>
+      <formula>$A141="begin repeat"</formula>
     </cfRule>
     <cfRule type="expression" priority="423" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="421">
-      <formula>$A142="end group"</formula>
+      <formula>$A141="end group"</formula>
     </cfRule>
     <cfRule type="expression" priority="424" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="422">
-      <formula>$A142="begin group"</formula>
+      <formula>$A141="begin group"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B146:B149">
@@ -37661,7 +37655,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A44" activeCellId="0" sqref="A44"/>
-      <selection pane="bottomRight" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="A3" activeCellId="1" sqref="P32:P36 A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.765625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -37676,33 +37670,33 @@
   <sheetData>
     <row r="1" s="8" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="B1" s="26" t="s">
         <v>203</v>
-      </c>
-      <c r="B1" s="26" t="s">
-        <v>204</v>
       </c>
       <c r="C1" s="27" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="26" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="28" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B2" s="29" t="n">
         <v>1</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D2" s="30"/>
       <c r="E2" s="31"/>
@@ -37710,13 +37704,13 @@
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="28" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B3" s="29" t="n">
         <v>1</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D3" s="30"/>
       <c r="E3" s="31"/>
@@ -37724,35 +37718,35 @@
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="28" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B4" s="28" t="n">
         <v>1</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="28" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B5" s="28" t="n">
         <v>1</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="28" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B6" s="28" t="n">
         <v>-1</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37768,7 +37762,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="32" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37779,7 +37773,7 @@
         <v>2</v>
       </c>
       <c r="C9" s="32" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37790,7 +37784,7 @@
         <v>3</v>
       </c>
       <c r="C10" s="32" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37801,7 +37795,7 @@
         <v>4</v>
       </c>
       <c r="C11" s="32" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -37812,111 +37806,111 @@
         <v>5</v>
       </c>
       <c r="C12" s="32" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="28" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B13" s="28" t="n">
         <v>0</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="28" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B14" s="28" t="s">
+        <v>221</v>
+      </c>
+      <c r="C14" s="33" t="s">
         <v>222</v>
-      </c>
-      <c r="C14" s="33" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="28" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B15" s="28" t="s">
+        <v>223</v>
+      </c>
+      <c r="C15" s="28" t="s">
         <v>224</v>
-      </c>
-      <c r="C15" s="28" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="28" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B16" s="28" t="s">
+        <v>225</v>
+      </c>
+      <c r="C16" s="28" t="s">
         <v>226</v>
-      </c>
-      <c r="C16" s="28" t="s">
-        <v>227</v>
       </c>
       <c r="H16" s="34"/>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="28" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B17" s="28" t="s">
+        <v>227</v>
+      </c>
+      <c r="C17" s="28" t="s">
         <v>228</v>
-      </c>
-      <c r="C17" s="28" t="s">
-        <v>229</v>
       </c>
       <c r="H17" s="34"/>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="28" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B18" s="28" t="s">
+        <v>229</v>
+      </c>
+      <c r="C18" s="28" t="s">
         <v>230</v>
-      </c>
-      <c r="C18" s="28" t="s">
-        <v>231</v>
       </c>
       <c r="H18" s="34"/>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="28" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B19" s="28" t="s">
+        <v>231</v>
+      </c>
+      <c r="C19" s="28" t="s">
         <v>232</v>
-      </c>
-      <c r="C19" s="28" t="s">
-        <v>233</v>
       </c>
       <c r="H19" s="34"/>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="28" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B20" s="28" t="s">
+        <v>233</v>
+      </c>
+      <c r="C20" s="33" t="s">
         <v>234</v>
-      </c>
-      <c r="C20" s="33" t="s">
-        <v>235</v>
       </c>
       <c r="H20" s="34"/>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="28" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B21" s="28" t="s">
+        <v>235</v>
+      </c>
+      <c r="C21" s="28" t="s">
         <v>236</v>
-      </c>
-      <c r="C21" s="28" t="s">
-        <v>237</v>
       </c>
       <c r="H21" s="34"/>
     </row>
@@ -39717,7 +39711,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="P32:P36 A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.765625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -39730,42 +39724,42 @@
   <sheetData>
     <row r="1" s="8" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="26" t="s">
+        <v>237</v>
+      </c>
+      <c r="B1" s="26" t="s">
         <v>238</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="C1" s="27" t="s">
         <v>239</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="D1" s="26" t="s">
         <v>240</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="E1" s="40" t="s">
         <v>241</v>
       </c>
-      <c r="E1" s="40" t="s">
+      <c r="F1" s="8" t="s">
         <v>242</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>243</v>
       </c>
       <c r="G1" s="41"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="24" t="s">
+        <v>243</v>
+      </c>
+      <c r="B2" s="24" t="s">
         <v>244</v>
-      </c>
-      <c r="B2" s="24" t="s">
-        <v>245</v>
       </c>
       <c r="C2" s="24" t="str">
         <f aca="true">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2306161019</v>
+        <v>2306161046</v>
       </c>
       <c r="D2" s="42"/>
       <c r="E2" s="24" t="s">
+        <v>245</v>
+      </c>
+      <c r="F2" s="25" t="s">
         <v>246</v>
-      </c>
-      <c r="F2" s="25" t="s">
-        <v>247</v>
       </c>
     </row>
   </sheetData>
@@ -39787,7 +39781,7 @@
   <dimension ref="A1:AD154"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A49" activeCellId="0" sqref="A49"/>
+      <selection pane="topLeft" activeCell="A49" activeCellId="1" sqref="P32:P36 A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -39799,7 +39793,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="43" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B1" s="43"/>
     </row>
@@ -39809,7 +39803,7 @@
     </row>
     <row r="3" customFormat="false" ht="96.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="45" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B3" s="45"/>
     </row>
@@ -39821,16 +39815,16 @@
         <v>1</v>
       </c>
       <c r="C5" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>250</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="E5" s="4" t="s">
         <v>251</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>252</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>253</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>5</v>
@@ -39842,10 +39836,10 @@
         <v>7</v>
       </c>
       <c r="J5" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="K5" s="7" t="s">
         <v>254</v>
-      </c>
-      <c r="K5" s="7" t="s">
-        <v>255</v>
       </c>
       <c r="L5" s="4" t="s">
         <v>9</v>
@@ -39857,10 +39851,10 @@
         <v>11</v>
       </c>
       <c r="O5" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="P5" s="4" t="s">
         <v>256</v>
-      </c>
-      <c r="P5" s="4" t="s">
-        <v>257</v>
       </c>
       <c r="Q5" s="4" t="s">
         <v>13</v>
@@ -39872,22 +39866,22 @@
         <v>16</v>
       </c>
       <c r="T5" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="U5" s="4" t="s">
         <v>258</v>
       </c>
-      <c r="U5" s="4" t="s">
+      <c r="V5" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="V5" s="4" t="s">
+      <c r="W5" s="4" t="s">
         <v>260</v>
       </c>
-      <c r="W5" s="4" t="s">
+      <c r="X5" s="4" t="s">
         <v>261</v>
       </c>
-      <c r="X5" s="4" t="s">
+      <c r="Y5" s="4" t="s">
         <v>262</v>
-      </c>
-      <c r="Y5" s="4" t="s">
-        <v>263</v>
       </c>
       <c r="Z5" s="4" t="s">
         <v>20</v>
@@ -39907,99 +39901,99 @@
     </row>
     <row r="6" s="48" customFormat="true" ht="189" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="47" t="s">
+        <v>263</v>
+      </c>
+      <c r="B6" s="47" t="s">
         <v>264</v>
       </c>
-      <c r="B6" s="47" t="s">
+      <c r="C6" s="47" t="s">
         <v>265</v>
       </c>
-      <c r="C6" s="47" t="s">
+      <c r="D6" s="47" t="s">
         <v>266</v>
       </c>
-      <c r="D6" s="47" t="s">
+      <c r="E6" s="47" t="s">
         <v>267</v>
       </c>
-      <c r="E6" s="47" t="s">
+      <c r="F6" s="47" t="s">
         <v>268</v>
       </c>
-      <c r="F6" s="47" t="s">
+      <c r="G6" s="47" t="s">
         <v>269</v>
       </c>
-      <c r="G6" s="47" t="s">
+      <c r="H6" s="47" t="s">
         <v>270</v>
       </c>
-      <c r="H6" s="47" t="s">
+      <c r="I6" s="47" t="s">
         <v>271</v>
       </c>
-      <c r="I6" s="47" t="s">
+      <c r="J6" s="47" t="s">
         <v>272</v>
       </c>
-      <c r="J6" s="47" t="s">
+      <c r="K6" s="47" t="s">
         <v>273</v>
       </c>
-      <c r="K6" s="47" t="s">
+      <c r="L6" s="47" t="s">
         <v>274</v>
       </c>
-      <c r="L6" s="47" t="s">
+      <c r="M6" s="47" t="s">
         <v>275</v>
       </c>
-      <c r="M6" s="47" t="s">
+      <c r="N6" s="47" t="s">
         <v>276</v>
       </c>
-      <c r="N6" s="47" t="s">
+      <c r="O6" s="47" t="s">
         <v>277</v>
       </c>
-      <c r="O6" s="47" t="s">
+      <c r="P6" s="47" t="s">
         <v>278</v>
       </c>
-      <c r="P6" s="47" t="s">
+      <c r="Q6" s="47" t="s">
         <v>279</v>
       </c>
-      <c r="Q6" s="47" t="s">
+      <c r="R6" s="47" t="s">
         <v>280</v>
       </c>
-      <c r="R6" s="47" t="s">
+      <c r="S6" s="47" t="s">
         <v>281</v>
       </c>
-      <c r="S6" s="47" t="s">
+      <c r="T6" s="47" t="s">
         <v>282</v>
       </c>
-      <c r="T6" s="47" t="s">
+      <c r="U6" s="47" t="s">
         <v>283</v>
       </c>
-      <c r="U6" s="47" t="s">
+      <c r="V6" s="47" t="s">
         <v>284</v>
       </c>
-      <c r="V6" s="47" t="s">
+      <c r="W6" s="47" t="s">
         <v>285</v>
       </c>
-      <c r="W6" s="47" t="s">
+      <c r="X6" s="47" t="s">
         <v>286</v>
       </c>
-      <c r="X6" s="47" t="s">
+      <c r="Y6" s="47" t="s">
         <v>287</v>
       </c>
-      <c r="Y6" s="47" t="s">
+      <c r="Z6" s="47" t="s">
         <v>288</v>
       </c>
-      <c r="Z6" s="47" t="s">
+      <c r="AA6" s="47" t="s">
         <v>289</v>
       </c>
-      <c r="AA6" s="47" t="s">
+      <c r="AB6" s="47" t="s">
         <v>290</v>
       </c>
-      <c r="AB6" s="47" t="s">
+      <c r="AC6" s="47" t="s">
         <v>291</v>
       </c>
-      <c r="AC6" s="47" t="s">
+      <c r="AD6" s="47" t="s">
         <v>292</v>
-      </c>
-      <c r="AD6" s="47" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="8" s="52" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="49" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B8" s="49"/>
       <c r="C8" s="50"/>
@@ -40033,13 +40027,13 @@
     </row>
     <row r="10" s="52" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="53" t="s">
+        <v>294</v>
+      </c>
+      <c r="B10" s="53" t="s">
         <v>295</v>
       </c>
-      <c r="B10" s="53" t="s">
+      <c r="C10" s="54" t="s">
         <v>296</v>
-      </c>
-      <c r="C10" s="54" t="s">
-        <v>297</v>
       </c>
       <c r="D10" s="53"/>
       <c r="E10" s="53"/>
@@ -40071,20 +40065,20 @@
     </row>
     <row r="11" s="52" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="53" t="s">
+        <v>294</v>
+      </c>
+      <c r="B11" s="53" t="s">
         <v>295</v>
       </c>
-      <c r="B11" s="53" t="s">
-        <v>296</v>
-      </c>
       <c r="C11" s="54" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D11" s="53"/>
       <c r="E11" s="53"/>
       <c r="F11" s="53"/>
       <c r="G11" s="53"/>
       <c r="H11" s="53" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="I11" s="53"/>
       <c r="J11" s="53"/>
@@ -40111,13 +40105,13 @@
     </row>
     <row r="12" s="52" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="53" t="s">
+        <v>299</v>
+      </c>
+      <c r="B12" s="53" t="s">
+        <v>295</v>
+      </c>
+      <c r="C12" s="54" t="s">
         <v>300</v>
-      </c>
-      <c r="B12" s="53" t="s">
-        <v>296</v>
-      </c>
-      <c r="C12" s="54" t="s">
-        <v>301</v>
       </c>
       <c r="D12" s="53"/>
       <c r="E12" s="53"/>
@@ -40149,13 +40143,13 @@
     </row>
     <row r="13" s="52" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="53" t="s">
+        <v>301</v>
+      </c>
+      <c r="B13" s="53" t="s">
+        <v>295</v>
+      </c>
+      <c r="C13" s="54" t="s">
         <v>302</v>
-      </c>
-      <c r="B13" s="53" t="s">
-        <v>296</v>
-      </c>
-      <c r="C13" s="54" t="s">
-        <v>303</v>
       </c>
       <c r="D13" s="53"/>
       <c r="E13" s="53"/>
@@ -40187,13 +40181,13 @@
     </row>
     <row r="14" s="52" customFormat="true" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="53" t="s">
+        <v>303</v>
+      </c>
+      <c r="B14" s="53" t="s">
+        <v>295</v>
+      </c>
+      <c r="C14" s="54" t="s">
         <v>304</v>
-      </c>
-      <c r="B14" s="53" t="s">
-        <v>296</v>
-      </c>
-      <c r="C14" s="54" t="s">
-        <v>305</v>
       </c>
       <c r="D14" s="53"/>
       <c r="E14" s="53"/>
@@ -40225,20 +40219,20 @@
     </row>
     <row r="15" s="52" customFormat="true" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="53" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B15" s="53" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C15" s="54" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D15" s="53"/>
       <c r="E15" s="53"/>
       <c r="F15" s="53"/>
       <c r="G15" s="53"/>
       <c r="H15" s="53" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="I15" s="53"/>
       <c r="J15" s="53"/>
@@ -40265,20 +40259,20 @@
     </row>
     <row r="16" s="52" customFormat="true" ht="63" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="53" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B16" s="53" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C16" s="54" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D16" s="53"/>
       <c r="E16" s="53"/>
       <c r="F16" s="53"/>
       <c r="G16" s="53"/>
       <c r="H16" s="53" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="I16" s="53"/>
       <c r="J16" s="53"/>
@@ -40305,20 +40299,20 @@
     </row>
     <row r="17" s="52" customFormat="true" ht="63" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="53" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B17" s="53" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C17" s="54" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D17" s="53"/>
       <c r="E17" s="53"/>
       <c r="F17" s="53"/>
       <c r="G17" s="53"/>
       <c r="H17" s="53" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="I17" s="53"/>
       <c r="J17" s="53"/>
@@ -40345,20 +40339,20 @@
     </row>
     <row r="18" s="52" customFormat="true" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="53" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B18" s="53" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C18" s="54" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D18" s="53"/>
       <c r="E18" s="53"/>
       <c r="F18" s="53"/>
       <c r="G18" s="53"/>
       <c r="H18" s="53" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="I18" s="53"/>
       <c r="J18" s="53"/>
@@ -40385,20 +40379,20 @@
     </row>
     <row r="19" s="52" customFormat="true" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="53" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B19" s="53" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C19" s="54" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D19" s="53"/>
       <c r="E19" s="53"/>
       <c r="F19" s="53"/>
       <c r="G19" s="53"/>
       <c r="H19" s="53" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="I19" s="53"/>
       <c r="J19" s="53"/>
@@ -40425,20 +40419,20 @@
     </row>
     <row r="20" s="52" customFormat="true" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="53" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B20" s="53" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C20" s="54" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D20" s="53"/>
       <c r="E20" s="53"/>
       <c r="F20" s="53"/>
       <c r="G20" s="53"/>
       <c r="H20" s="53" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="I20" s="53"/>
       <c r="J20" s="53"/>
@@ -40465,20 +40459,20 @@
     </row>
     <row r="21" s="52" customFormat="true" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="53" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B21" s="53" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C21" s="54" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D21" s="53"/>
       <c r="E21" s="53"/>
       <c r="F21" s="53"/>
       <c r="G21" s="53"/>
       <c r="H21" s="53" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="I21" s="53"/>
       <c r="J21" s="53"/>
@@ -40505,20 +40499,20 @@
     </row>
     <row r="22" s="52" customFormat="true" ht="63" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="53" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B22" s="53" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C22" s="54" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D22" s="53"/>
       <c r="E22" s="53"/>
       <c r="F22" s="53"/>
       <c r="G22" s="53"/>
       <c r="H22" s="53" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I22" s="53"/>
       <c r="J22" s="53"/>
@@ -40545,20 +40539,20 @@
     </row>
     <row r="23" s="52" customFormat="true" ht="78.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="53" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B23" s="53" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C23" s="54" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D23" s="53"/>
       <c r="E23" s="53"/>
       <c r="F23" s="53"/>
       <c r="G23" s="53"/>
       <c r="H23" s="53" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="I23" s="53"/>
       <c r="J23" s="53"/>
@@ -40585,20 +40579,20 @@
     </row>
     <row r="24" s="52" customFormat="true" ht="63" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="53" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B24" s="53" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C24" s="54" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D24" s="53"/>
       <c r="E24" s="53"/>
       <c r="F24" s="53"/>
       <c r="G24" s="53"/>
       <c r="H24" s="53" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="I24" s="53"/>
       <c r="J24" s="53"/>
@@ -40625,20 +40619,20 @@
     </row>
     <row r="25" s="52" customFormat="true" ht="63" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="53" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B25" s="53" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C25" s="54" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D25" s="53"/>
       <c r="E25" s="53"/>
       <c r="F25" s="53"/>
       <c r="G25" s="53"/>
       <c r="H25" s="53" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="I25" s="53"/>
       <c r="J25" s="53"/>
@@ -40665,20 +40659,20 @@
     </row>
     <row r="26" s="52" customFormat="true" ht="63" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="53" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B26" s="53" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C26" s="55" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D26" s="53"/>
       <c r="E26" s="53"/>
       <c r="F26" s="53"/>
       <c r="G26" s="53"/>
       <c r="H26" s="53" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="I26" s="53"/>
       <c r="J26" s="53"/>
@@ -40705,20 +40699,20 @@
     </row>
     <row r="27" s="52" customFormat="true" ht="63" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="53" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B27" s="53" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C27" s="54" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D27" s="53"/>
       <c r="E27" s="53"/>
       <c r="F27" s="53"/>
       <c r="G27" s="53"/>
       <c r="H27" s="53" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="I27" s="53"/>
       <c r="J27" s="53"/>
@@ -40745,20 +40739,20 @@
     </row>
     <row r="28" s="52" customFormat="true" ht="78.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="53" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B28" s="53" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C28" s="54" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D28" s="53"/>
       <c r="E28" s="53"/>
       <c r="F28" s="53"/>
       <c r="G28" s="53"/>
       <c r="H28" s="53" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="I28" s="53"/>
       <c r="J28" s="53"/>
@@ -40785,13 +40779,13 @@
     </row>
     <row r="29" s="52" customFormat="true" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="53" t="s">
+        <v>333</v>
+      </c>
+      <c r="B29" s="53" t="s">
+        <v>295</v>
+      </c>
+      <c r="C29" s="54" t="s">
         <v>334</v>
-      </c>
-      <c r="B29" s="53" t="s">
-        <v>296</v>
-      </c>
-      <c r="C29" s="54" t="s">
-        <v>335</v>
       </c>
       <c r="D29" s="53"/>
       <c r="E29" s="53"/>
@@ -40823,20 +40817,20 @@
     </row>
     <row r="30" s="52" customFormat="true" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="53" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B30" s="53" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C30" s="54" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D30" s="53"/>
       <c r="E30" s="53"/>
       <c r="F30" s="53"/>
       <c r="G30" s="53"/>
       <c r="H30" s="53" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="I30" s="53"/>
       <c r="J30" s="53"/>
@@ -40863,20 +40857,20 @@
     </row>
     <row r="31" s="52" customFormat="true" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="53" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B31" s="53" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C31" s="54" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D31" s="53"/>
       <c r="E31" s="53"/>
       <c r="F31" s="53"/>
       <c r="G31" s="53"/>
       <c r="H31" s="53" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="I31" s="53"/>
       <c r="J31" s="53"/>
@@ -40903,20 +40897,20 @@
     </row>
     <row r="32" s="52" customFormat="true" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="53" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B32" s="53" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C32" s="54" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D32" s="53"/>
       <c r="E32" s="53"/>
       <c r="F32" s="53"/>
       <c r="G32" s="53"/>
       <c r="H32" s="53" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="I32" s="53"/>
       <c r="J32" s="53"/>
@@ -40943,20 +40937,20 @@
     </row>
     <row r="33" s="52" customFormat="true" ht="63" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="53" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B33" s="53" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C33" s="54" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D33" s="53"/>
       <c r="E33" s="53"/>
       <c r="F33" s="53"/>
       <c r="G33" s="53"/>
       <c r="H33" s="53" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="I33" s="53"/>
       <c r="J33" s="53"/>
@@ -40983,20 +40977,20 @@
     </row>
     <row r="34" s="52" customFormat="true" ht="63" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="53" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B34" s="53" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C34" s="54" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D34" s="53"/>
       <c r="E34" s="53"/>
       <c r="F34" s="53"/>
       <c r="G34" s="53"/>
       <c r="H34" s="53" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="I34" s="53"/>
       <c r="J34" s="53"/>
@@ -41023,20 +41017,20 @@
     </row>
     <row r="35" s="52" customFormat="true" ht="63" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="53" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B35" s="53" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C35" s="55" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D35" s="53"/>
       <c r="E35" s="53"/>
       <c r="F35" s="53"/>
       <c r="G35" s="53"/>
       <c r="H35" s="53" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="I35" s="53"/>
       <c r="J35" s="53"/>
@@ -41063,20 +41057,20 @@
     </row>
     <row r="36" s="52" customFormat="true" ht="63" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="53" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B36" s="53" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C36" s="54" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D36" s="53"/>
       <c r="E36" s="53"/>
       <c r="F36" s="53"/>
       <c r="G36" s="53"/>
       <c r="H36" s="53" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="I36" s="53"/>
       <c r="J36" s="53"/>
@@ -41103,20 +41097,20 @@
     </row>
     <row r="37" s="52" customFormat="true" ht="78.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="53" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B37" s="53" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C37" s="54" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D37" s="53"/>
       <c r="E37" s="53"/>
       <c r="F37" s="53"/>
       <c r="G37" s="53"/>
       <c r="H37" s="53" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="I37" s="53"/>
       <c r="J37" s="53"/>
@@ -41143,13 +41137,13 @@
     </row>
     <row r="38" s="52" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="53" t="s">
+        <v>343</v>
+      </c>
+      <c r="B38" s="53" t="s">
+        <v>295</v>
+      </c>
+      <c r="C38" s="54" t="s">
         <v>344</v>
-      </c>
-      <c r="B38" s="53" t="s">
-        <v>296</v>
-      </c>
-      <c r="C38" s="54" t="s">
-        <v>345</v>
       </c>
       <c r="D38" s="53"/>
       <c r="E38" s="53"/>
@@ -41181,13 +41175,13 @@
     </row>
     <row r="39" s="52" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="53" t="s">
+        <v>345</v>
+      </c>
+      <c r="B39" s="53" t="s">
+        <v>295</v>
+      </c>
+      <c r="C39" s="54" t="s">
         <v>346</v>
-      </c>
-      <c r="B39" s="53" t="s">
-        <v>296</v>
-      </c>
-      <c r="C39" s="54" t="s">
-        <v>347</v>
       </c>
       <c r="D39" s="53"/>
       <c r="E39" s="53"/>
@@ -41219,13 +41213,13 @@
     </row>
     <row r="40" s="52" customFormat="true" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="53" t="s">
+        <v>347</v>
+      </c>
+      <c r="B40" s="53" t="s">
+        <v>295</v>
+      </c>
+      <c r="C40" s="54" t="s">
         <v>348</v>
-      </c>
-      <c r="B40" s="53" t="s">
-        <v>296</v>
-      </c>
-      <c r="C40" s="54" t="s">
-        <v>349</v>
       </c>
       <c r="D40" s="53"/>
       <c r="E40" s="53"/>
@@ -41257,13 +41251,13 @@
     </row>
     <row r="41" s="52" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="53" t="s">
+        <v>349</v>
+      </c>
+      <c r="B41" s="53" t="s">
+        <v>295</v>
+      </c>
+      <c r="C41" s="54" t="s">
         <v>350</v>
-      </c>
-      <c r="B41" s="53" t="s">
-        <v>296</v>
-      </c>
-      <c r="C41" s="54" t="s">
-        <v>351</v>
       </c>
       <c r="D41" s="53"/>
       <c r="E41" s="53"/>
@@ -41298,10 +41292,10 @@
         <v>45</v>
       </c>
       <c r="B42" s="53" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C42" s="54" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D42" s="53"/>
       <c r="E42" s="53"/>
@@ -41336,17 +41330,17 @@
         <v>45</v>
       </c>
       <c r="B43" s="53" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C43" s="54" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D43" s="53"/>
       <c r="E43" s="53"/>
       <c r="F43" s="53"/>
       <c r="G43" s="53"/>
       <c r="H43" s="53" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="I43" s="53"/>
       <c r="J43" s="53"/>
@@ -41373,13 +41367,13 @@
     </row>
     <row r="44" s="52" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="53" t="s">
+        <v>354</v>
+      </c>
+      <c r="B44" s="53" t="s">
+        <v>295</v>
+      </c>
+      <c r="C44" s="54" t="s">
         <v>355</v>
-      </c>
-      <c r="B44" s="53" t="s">
-        <v>296</v>
-      </c>
-      <c r="C44" s="54" t="s">
-        <v>356</v>
       </c>
       <c r="D44" s="53"/>
       <c r="E44" s="53"/>
@@ -41411,20 +41405,20 @@
     </row>
     <row r="45" s="52" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="53" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B45" s="53" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C45" s="54" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D45" s="53"/>
       <c r="E45" s="53"/>
       <c r="F45" s="53"/>
       <c r="G45" s="53"/>
       <c r="H45" s="53" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="I45" s="53"/>
       <c r="J45" s="53"/>
@@ -41451,13 +41445,13 @@
     </row>
     <row r="46" s="52" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="53" t="s">
+        <v>357</v>
+      </c>
+      <c r="B46" s="53" t="s">
+        <v>295</v>
+      </c>
+      <c r="C46" s="54" t="s">
         <v>358</v>
-      </c>
-      <c r="B46" s="53" t="s">
-        <v>296</v>
-      </c>
-      <c r="C46" s="54" t="s">
-        <v>359</v>
       </c>
       <c r="D46" s="53"/>
       <c r="E46" s="53"/>
@@ -41489,20 +41483,20 @@
     </row>
     <row r="47" s="52" customFormat="true" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="53" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B47" s="53" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C47" s="54" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D47" s="53"/>
       <c r="E47" s="53"/>
       <c r="F47" s="53"/>
       <c r="G47" s="53"/>
       <c r="H47" s="53" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="I47" s="53"/>
       <c r="J47" s="53"/>
@@ -41529,20 +41523,20 @@
     </row>
     <row r="48" s="52" customFormat="true" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="53" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B48" s="53" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C48" s="54" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D48" s="53"/>
       <c r="E48" s="53"/>
       <c r="F48" s="53"/>
       <c r="G48" s="53"/>
       <c r="H48" s="53" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="I48" s="53"/>
       <c r="J48" s="53"/>
@@ -41569,20 +41563,20 @@
     </row>
     <row r="49" s="52" customFormat="true" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="53" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B49" s="53" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C49" s="54" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D49" s="53"/>
       <c r="E49" s="53"/>
       <c r="F49" s="53"/>
       <c r="G49" s="53"/>
       <c r="H49" s="53" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="I49" s="53"/>
       <c r="J49" s="53"/>
@@ -41609,13 +41603,13 @@
     </row>
     <row r="50" s="52" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="53" t="s">
+        <v>365</v>
+      </c>
+      <c r="B50" s="53" t="s">
+        <v>295</v>
+      </c>
+      <c r="C50" s="54" t="s">
         <v>366</v>
-      </c>
-      <c r="B50" s="53" t="s">
-        <v>296</v>
-      </c>
-      <c r="C50" s="54" t="s">
-        <v>367</v>
       </c>
       <c r="D50" s="53"/>
       <c r="E50" s="53"/>
@@ -41647,13 +41641,13 @@
     </row>
     <row r="51" s="52" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="53" t="s">
+        <v>367</v>
+      </c>
+      <c r="B51" s="53" t="s">
+        <v>295</v>
+      </c>
+      <c r="C51" s="54" t="s">
         <v>368</v>
-      </c>
-      <c r="B51" s="53" t="s">
-        <v>296</v>
-      </c>
-      <c r="C51" s="54" t="s">
-        <v>369</v>
       </c>
       <c r="D51" s="53"/>
       <c r="E51" s="53"/>
@@ -41685,13 +41679,13 @@
     </row>
     <row r="52" s="52" customFormat="true" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="53" t="s">
+        <v>369</v>
+      </c>
+      <c r="B52" s="53" t="s">
+        <v>295</v>
+      </c>
+      <c r="C52" s="54" t="s">
         <v>370</v>
-      </c>
-      <c r="B52" s="53" t="s">
-        <v>296</v>
-      </c>
-      <c r="C52" s="54" t="s">
-        <v>371</v>
       </c>
       <c r="D52" s="53"/>
       <c r="E52" s="53"/>
@@ -41726,10 +41720,10 @@
         <v>22</v>
       </c>
       <c r="B53" s="53" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C53" s="54" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D53" s="53"/>
       <c r="E53" s="53"/>
@@ -41761,10 +41755,10 @@
     </row>
     <row r="54" s="52" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="53" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B54" s="53" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C54" s="54"/>
       <c r="D54" s="53"/>
@@ -41797,10 +41791,10 @@
     </row>
     <row r="55" s="52" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="53" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B55" s="53" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C55" s="54"/>
       <c r="D55" s="53"/>
@@ -41833,10 +41827,10 @@
     </row>
     <row r="56" s="52" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="53" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B56" s="53" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C56" s="54"/>
       <c r="D56" s="53"/>
@@ -41869,10 +41863,10 @@
     </row>
     <row r="57" s="52" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="53" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B57" s="53" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C57" s="54"/>
       <c r="D57" s="53"/>
@@ -41905,10 +41899,10 @@
     </row>
     <row r="58" s="52" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="53" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B58" s="53" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C58" s="54"/>
       <c r="D58" s="53"/>
@@ -41941,10 +41935,10 @@
     </row>
     <row r="59" s="52" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="53" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B59" s="53" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C59" s="54"/>
       <c r="D59" s="53"/>
@@ -41977,10 +41971,10 @@
     </row>
     <row r="60" s="52" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="53" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B60" s="53" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C60" s="54"/>
       <c r="D60" s="53"/>
@@ -42013,10 +42007,10 @@
     </row>
     <row r="61" s="52" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="53" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B61" s="53" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C61" s="54"/>
       <c r="D61" s="53"/>
@@ -42052,7 +42046,7 @@
         <v>58</v>
       </c>
       <c r="B62" s="53" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C62" s="54"/>
       <c r="D62" s="53"/>
@@ -42070,7 +42064,7 @@
       <c r="P62" s="53"/>
       <c r="Q62" s="53"/>
       <c r="R62" s="53" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="S62" s="53"/>
       <c r="T62" s="53"/>
@@ -42087,10 +42081,10 @@
     </row>
     <row r="63" s="52" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="53" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B63" s="53" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C63" s="54"/>
       <c r="D63" s="53"/>
@@ -42108,7 +42102,7 @@
       <c r="P63" s="53"/>
       <c r="Q63" s="53"/>
       <c r="R63" s="53" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="S63" s="53"/>
       <c r="T63" s="53"/>
@@ -42125,10 +42119,10 @@
     </row>
     <row r="64" s="52" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="53" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B64" s="53" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C64" s="54"/>
       <c r="D64" s="53"/>
@@ -42136,7 +42130,7 @@
       <c r="F64" s="53"/>
       <c r="G64" s="53"/>
       <c r="H64" s="53" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="I64" s="53"/>
       <c r="J64" s="53"/>
@@ -42163,10 +42157,10 @@
     </row>
     <row r="65" s="52" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="53" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B65" s="53" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C65" s="54"/>
       <c r="D65" s="53"/>
@@ -42174,7 +42168,7 @@
       <c r="F65" s="53"/>
       <c r="G65" s="53"/>
       <c r="H65" s="53" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="I65" s="53"/>
       <c r="J65" s="53"/>
@@ -42201,10 +42195,10 @@
     </row>
     <row r="66" s="52" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="53" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B66" s="53" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C66" s="54"/>
       <c r="D66" s="53"/>
@@ -42212,7 +42206,7 @@
       <c r="F66" s="53"/>
       <c r="G66" s="53"/>
       <c r="H66" s="53" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="I66" s="53"/>
       <c r="J66" s="53"/>
@@ -42239,10 +42233,10 @@
     </row>
     <row r="67" s="52" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="53" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B67" s="53" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C67" s="54"/>
       <c r="D67" s="53"/>
@@ -42250,7 +42244,7 @@
       <c r="F67" s="53"/>
       <c r="G67" s="53"/>
       <c r="H67" s="53" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="I67" s="53"/>
       <c r="J67" s="53"/>
@@ -42280,10 +42274,10 @@
         <v>26</v>
       </c>
       <c r="B68" s="53" t="s">
+        <v>389</v>
+      </c>
+      <c r="C68" s="54" t="s">
         <v>390</v>
-      </c>
-      <c r="C68" s="54" t="s">
-        <v>391</v>
       </c>
       <c r="D68" s="53"/>
       <c r="E68" s="53"/>
@@ -42315,7 +42309,7 @@
     </row>
     <row r="69" s="52" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="53" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B69" s="53"/>
       <c r="C69" s="54"/>
@@ -42352,7 +42346,7 @@
         <v>57</v>
       </c>
       <c r="B70" s="53" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C70" s="54"/>
       <c r="D70" s="53"/>
@@ -42385,13 +42379,13 @@
     </row>
     <row r="71" s="52" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="53" t="s">
+        <v>392</v>
+      </c>
+      <c r="B71" s="53" t="s">
         <v>393</v>
       </c>
-      <c r="B71" s="53" t="s">
+      <c r="C71" s="54" t="s">
         <v>394</v>
-      </c>
-      <c r="C71" s="54" t="s">
-        <v>395</v>
       </c>
       <c r="D71" s="53"/>
       <c r="E71" s="53"/>
@@ -42423,7 +42417,7 @@
     </row>
     <row r="72" s="52" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="53" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B72" s="53"/>
       <c r="C72" s="54"/>
@@ -42457,10 +42451,10 @@
     </row>
     <row r="73" s="52" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="53" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B73" s="53" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C73" s="54"/>
       <c r="D73" s="53"/>
@@ -42493,13 +42487,13 @@
     </row>
     <row r="74" s="52" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="53" t="s">
+        <v>392</v>
+      </c>
+      <c r="B74" s="53" t="s">
         <v>393</v>
       </c>
-      <c r="B74" s="53" t="s">
-        <v>394</v>
-      </c>
       <c r="C74" s="54" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D74" s="53"/>
       <c r="E74" s="53"/>
@@ -42533,7 +42527,7 @@
     </row>
     <row r="75" s="52" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="53" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B75" s="53"/>
       <c r="C75" s="54"/>
@@ -42567,10 +42561,10 @@
     </row>
     <row r="76" s="52" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="53" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B76" s="53" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C76" s="54"/>
       <c r="D76" s="53"/>
@@ -42603,10 +42597,10 @@
     </row>
     <row r="77" s="52" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="53" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B77" s="53" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C77" s="54"/>
       <c r="D77" s="53"/>
@@ -42639,10 +42633,10 @@
     </row>
     <row r="78" s="52" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="53" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B78" s="53" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C78" s="54"/>
       <c r="D78" s="53"/>
@@ -42675,10 +42669,10 @@
     </row>
     <row r="79" s="52" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="53" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B79" s="53" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C79" s="54"/>
       <c r="D79" s="53"/>
@@ -42686,7 +42680,7 @@
       <c r="F79" s="53"/>
       <c r="G79" s="53"/>
       <c r="H79" s="53" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="I79" s="53"/>
       <c r="J79" s="53"/>
@@ -42713,10 +42707,10 @@
     </row>
     <row r="80" s="52" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="53" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B80" s="53" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C80" s="54"/>
       <c r="D80" s="53"/>
@@ -42724,7 +42718,7 @@
       <c r="F80" s="53"/>
       <c r="G80" s="53"/>
       <c r="H80" s="53" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="I80" s="53"/>
       <c r="J80" s="53"/>
@@ -42751,10 +42745,10 @@
     </row>
     <row r="81" s="52" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="53" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B81" s="53" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C81" s="54"/>
       <c r="D81" s="53"/>
@@ -42762,7 +42756,7 @@
       <c r="F81" s="53"/>
       <c r="G81" s="53"/>
       <c r="H81" s="53" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="I81" s="53"/>
       <c r="J81" s="53"/>
@@ -42789,7 +42783,7 @@
     </row>
     <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="57" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B83" s="57"/>
       <c r="C83" s="58"/>
@@ -42823,27 +42817,27 @@
     </row>
     <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="60" t="s">
+        <v>406</v>
+      </c>
+      <c r="B85" s="60" t="s">
         <v>407</v>
       </c>
-      <c r="B85" s="60" t="s">
+      <c r="C85" s="60" t="s">
         <v>408</v>
       </c>
-      <c r="C85" s="60" t="s">
+      <c r="D85" s="60" t="s">
         <v>409</v>
-      </c>
-      <c r="D85" s="60" t="s">
-        <v>410</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="61" t="s">
+        <v>410</v>
+      </c>
+      <c r="B86" s="61" t="s">
         <v>411</v>
       </c>
-      <c r="B86" s="61" t="s">
+      <c r="C86" s="61" t="s">
         <v>412</v>
-      </c>
-      <c r="C86" s="61" t="s">
-        <v>413</v>
       </c>
       <c r="D86" s="61" t="n">
         <v>2</v>
@@ -42851,10 +42845,10 @@
     </row>
     <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="61" t="s">
+        <v>413</v>
+      </c>
+      <c r="B87" s="61" t="s">
         <v>414</v>
-      </c>
-      <c r="B87" s="61" t="s">
-        <v>415</v>
       </c>
       <c r="C87" s="62" t="str">
         <f aca="false">"3 - 2"</f>
@@ -42866,13 +42860,13 @@
     </row>
     <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="61" t="s">
+        <v>415</v>
+      </c>
+      <c r="B88" s="61" t="s">
         <v>416</v>
       </c>
-      <c r="B88" s="61" t="s">
+      <c r="C88" s="61" t="s">
         <v>417</v>
-      </c>
-      <c r="C88" s="61" t="s">
-        <v>418</v>
       </c>
       <c r="D88" s="61" t="n">
         <v>6</v>
@@ -42880,13 +42874,13 @@
     </row>
     <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="61" t="s">
+        <v>418</v>
+      </c>
+      <c r="B89" s="61" t="s">
         <v>419</v>
       </c>
-      <c r="B89" s="61" t="s">
+      <c r="C89" s="61" t="s">
         <v>420</v>
-      </c>
-      <c r="C89" s="61" t="s">
-        <v>421</v>
       </c>
       <c r="D89" s="61" t="n">
         <v>5</v>
@@ -42894,13 +42888,13 @@
     </row>
     <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="61" t="s">
+        <v>421</v>
+      </c>
+      <c r="B90" s="61" t="s">
         <v>422</v>
       </c>
-      <c r="B90" s="61" t="s">
+      <c r="C90" s="61" t="s">
         <v>423</v>
-      </c>
-      <c r="C90" s="61" t="s">
-        <v>424</v>
       </c>
       <c r="D90" s="61" t="n">
         <v>1</v>
@@ -42908,128 +42902,128 @@
     </row>
     <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="61" t="s">
+        <v>424</v>
+      </c>
+      <c r="B91" s="61" t="s">
         <v>425</v>
       </c>
-      <c r="B91" s="61" t="s">
+      <c r="C91" s="61" t="s">
         <v>426</v>
       </c>
-      <c r="C91" s="61" t="s">
+      <c r="D91" s="61" t="s">
         <v>427</v>
-      </c>
-      <c r="D91" s="61" t="s">
-        <v>428</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="61" t="s">
+        <v>428</v>
+      </c>
+      <c r="B92" s="61" t="s">
         <v>429</v>
       </c>
-      <c r="B92" s="61" t="s">
+      <c r="C92" s="61" t="s">
         <v>430</v>
       </c>
-      <c r="C92" s="61" t="s">
-        <v>431</v>
-      </c>
       <c r="D92" s="61" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="61" t="s">
+        <v>431</v>
+      </c>
+      <c r="B93" s="61" t="s">
         <v>432</v>
       </c>
-      <c r="B93" s="61" t="s">
+      <c r="C93" s="61" t="s">
         <v>433</v>
       </c>
-      <c r="C93" s="61" t="s">
-        <v>434</v>
-      </c>
       <c r="D93" s="61" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="61" t="s">
+        <v>434</v>
+      </c>
+      <c r="B94" s="61" t="s">
         <v>435</v>
       </c>
-      <c r="B94" s="61" t="s">
+      <c r="C94" s="61" t="s">
         <v>436</v>
       </c>
-      <c r="C94" s="61" t="s">
-        <v>437</v>
-      </c>
       <c r="D94" s="61" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="61" t="s">
+        <v>437</v>
+      </c>
+      <c r="B95" s="61" t="s">
         <v>438</v>
       </c>
-      <c r="B95" s="61" t="s">
+      <c r="C95" s="61" t="s">
         <v>439</v>
       </c>
-      <c r="C95" s="61" t="s">
-        <v>440</v>
-      </c>
       <c r="D95" s="61" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="61" t="s">
+        <v>440</v>
+      </c>
+      <c r="B96" s="61" t="s">
         <v>441</v>
       </c>
-      <c r="B96" s="61" t="s">
+      <c r="C96" s="61" t="s">
         <v>442</v>
       </c>
-      <c r="C96" s="61" t="s">
-        <v>443</v>
-      </c>
       <c r="D96" s="61" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="61" t="s">
+        <v>443</v>
+      </c>
+      <c r="B97" s="61" t="s">
         <v>444</v>
       </c>
-      <c r="B97" s="61" t="s">
+      <c r="C97" s="61" t="s">
         <v>445</v>
       </c>
-      <c r="C97" s="61" t="s">
-        <v>446</v>
-      </c>
       <c r="D97" s="61" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="61" t="s">
+        <v>446</v>
+      </c>
+      <c r="B98" s="61" t="s">
         <v>447</v>
       </c>
-      <c r="B98" s="61" t="s">
+      <c r="C98" s="61" t="s">
         <v>448</v>
       </c>
-      <c r="C98" s="61" t="s">
-        <v>449</v>
-      </c>
       <c r="D98" s="61" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="61" t="s">
+        <v>449</v>
+      </c>
+      <c r="B99" s="61" t="s">
         <v>450</v>
       </c>
-      <c r="B99" s="61" t="s">
+      <c r="C99" s="61" t="s">
         <v>451</v>
       </c>
-      <c r="C99" s="61" t="s">
+      <c r="D99" s="61" t="s">
         <v>452</v>
-      </c>
-      <c r="D99" s="61" t="s">
-        <v>453</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -43041,540 +43035,540 @@
     <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="59"/>
       <c r="B101" s="60" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C101" s="60" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D101" s="59"/>
     </row>
     <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="59"/>
       <c r="B102" s="63" t="s">
+        <v>454</v>
+      </c>
+      <c r="C102" s="64" t="s">
         <v>455</v>
-      </c>
-      <c r="C102" s="64" t="s">
-        <v>456</v>
       </c>
       <c r="D102" s="59"/>
     </row>
     <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="59"/>
       <c r="B103" s="64" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C103" s="64" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D103" s="59"/>
     </row>
     <row r="104" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="59"/>
       <c r="B104" s="64" t="s">
+        <v>456</v>
+      </c>
+      <c r="C104" s="64" t="s">
         <v>457</v>
-      </c>
-      <c r="C104" s="64" t="s">
-        <v>458</v>
       </c>
       <c r="D104" s="59"/>
     </row>
     <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="59"/>
       <c r="B105" s="64" t="s">
+        <v>458</v>
+      </c>
+      <c r="C105" s="64" t="s">
         <v>459</v>
-      </c>
-      <c r="C105" s="64" t="s">
-        <v>460</v>
       </c>
       <c r="D105" s="59"/>
     </row>
     <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="59"/>
       <c r="B106" s="64" t="s">
+        <v>460</v>
+      </c>
+      <c r="C106" s="64" t="s">
         <v>461</v>
-      </c>
-      <c r="C106" s="64" t="s">
-        <v>462</v>
       </c>
       <c r="D106" s="59"/>
     </row>
     <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="59"/>
       <c r="B107" s="64" t="s">
+        <v>462</v>
+      </c>
+      <c r="C107" s="64" t="s">
         <v>463</v>
-      </c>
-      <c r="C107" s="64" t="s">
-        <v>464</v>
       </c>
       <c r="D107" s="59"/>
     </row>
     <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="59"/>
       <c r="B108" s="64" t="s">
+        <v>464</v>
+      </c>
+      <c r="C108" s="64" t="s">
         <v>465</v>
-      </c>
-      <c r="C108" s="64" t="s">
-        <v>466</v>
       </c>
       <c r="D108" s="59"/>
     </row>
     <row r="109" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="59"/>
       <c r="B109" s="64" t="s">
+        <v>466</v>
+      </c>
+      <c r="C109" s="64" t="s">
         <v>467</v>
-      </c>
-      <c r="C109" s="64" t="s">
-        <v>468</v>
       </c>
       <c r="D109" s="59"/>
     </row>
     <row r="110" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="59"/>
       <c r="B110" s="64" t="s">
+        <v>468</v>
+      </c>
+      <c r="C110" s="64" t="s">
         <v>469</v>
-      </c>
-      <c r="C110" s="64" t="s">
-        <v>470</v>
       </c>
       <c r="D110" s="59"/>
     </row>
     <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="59"/>
       <c r="B111" s="64" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C111" s="64" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="D111" s="59"/>
     </row>
     <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="59"/>
       <c r="B112" s="64" t="s">
+        <v>471</v>
+      </c>
+      <c r="C112" s="64" t="s">
         <v>472</v>
-      </c>
-      <c r="C112" s="64" t="s">
-        <v>473</v>
       </c>
       <c r="D112" s="59"/>
     </row>
     <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="59"/>
       <c r="B113" s="64" t="s">
+        <v>473</v>
+      </c>
+      <c r="C113" s="64" t="s">
         <v>474</v>
-      </c>
-      <c r="C113" s="64" t="s">
-        <v>475</v>
       </c>
       <c r="D113" s="59"/>
     </row>
     <row r="114" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="59"/>
       <c r="B114" s="64" t="s">
+        <v>475</v>
+      </c>
+      <c r="C114" s="64" t="s">
         <v>476</v>
-      </c>
-      <c r="C114" s="64" t="s">
-        <v>477</v>
       </c>
       <c r="D114" s="59"/>
     </row>
     <row r="115" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="59"/>
       <c r="B115" s="64" t="s">
+        <v>477</v>
+      </c>
+      <c r="C115" s="64" t="s">
         <v>478</v>
-      </c>
-      <c r="C115" s="64" t="s">
-        <v>479</v>
       </c>
       <c r="D115" s="59"/>
     </row>
     <row r="116" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="59"/>
       <c r="B116" s="64" t="s">
+        <v>479</v>
+      </c>
+      <c r="C116" s="64" t="s">
         <v>480</v>
-      </c>
-      <c r="C116" s="64" t="s">
-        <v>481</v>
       </c>
       <c r="D116" s="59"/>
     </row>
     <row r="117" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="59"/>
       <c r="B117" s="64" t="s">
+        <v>481</v>
+      </c>
+      <c r="C117" s="64" t="s">
         <v>482</v>
-      </c>
-      <c r="C117" s="64" t="s">
-        <v>483</v>
       </c>
       <c r="D117" s="59"/>
     </row>
     <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="59"/>
       <c r="B118" s="64" t="s">
+        <v>483</v>
+      </c>
+      <c r="C118" s="64" t="s">
         <v>484</v>
-      </c>
-      <c r="C118" s="64" t="s">
-        <v>485</v>
       </c>
       <c r="D118" s="59"/>
     </row>
     <row r="119" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="59"/>
       <c r="B119" s="64" t="s">
+        <v>485</v>
+      </c>
+      <c r="C119" s="64" t="s">
         <v>486</v>
-      </c>
-      <c r="C119" s="64" t="s">
-        <v>487</v>
       </c>
       <c r="D119" s="59"/>
     </row>
     <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="59"/>
       <c r="B120" s="64" t="s">
+        <v>487</v>
+      </c>
+      <c r="C120" s="64" t="s">
         <v>488</v>
-      </c>
-      <c r="C120" s="64" t="s">
-        <v>489</v>
       </c>
       <c r="D120" s="59"/>
     </row>
     <row r="121" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="59"/>
       <c r="B121" s="64" t="s">
+        <v>489</v>
+      </c>
+      <c r="C121" s="64" t="s">
         <v>490</v>
-      </c>
-      <c r="C121" s="64" t="s">
-        <v>491</v>
       </c>
       <c r="D121" s="59"/>
     </row>
     <row r="122" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="59"/>
       <c r="B122" s="64" t="s">
+        <v>491</v>
+      </c>
+      <c r="C122" s="64" t="s">
         <v>492</v>
-      </c>
-      <c r="C122" s="64" t="s">
-        <v>493</v>
       </c>
       <c r="D122" s="59"/>
     </row>
     <row r="123" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="59"/>
       <c r="B123" s="64" t="s">
+        <v>493</v>
+      </c>
+      <c r="C123" s="64" t="s">
         <v>494</v>
-      </c>
-      <c r="C123" s="64" t="s">
-        <v>495</v>
       </c>
       <c r="D123" s="59"/>
     </row>
     <row r="124" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="59"/>
       <c r="B124" s="64" t="s">
+        <v>495</v>
+      </c>
+      <c r="C124" s="64" t="s">
         <v>496</v>
-      </c>
-      <c r="C124" s="64" t="s">
-        <v>497</v>
       </c>
       <c r="D124" s="59"/>
     </row>
     <row r="125" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="59"/>
       <c r="B125" s="64" t="s">
+        <v>497</v>
+      </c>
+      <c r="C125" s="64" t="s">
         <v>498</v>
-      </c>
-      <c r="C125" s="64" t="s">
-        <v>499</v>
       </c>
       <c r="D125" s="59"/>
     </row>
     <row r="126" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="59"/>
       <c r="B126" s="64" t="s">
+        <v>499</v>
+      </c>
+      <c r="C126" s="64" t="s">
         <v>500</v>
-      </c>
-      <c r="C126" s="64" t="s">
-        <v>501</v>
       </c>
       <c r="D126" s="59"/>
     </row>
     <row r="127" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="59"/>
       <c r="B127" s="64" t="s">
+        <v>501</v>
+      </c>
+      <c r="C127" s="64" t="s">
         <v>502</v>
-      </c>
-      <c r="C127" s="64" t="s">
-        <v>503</v>
       </c>
       <c r="D127" s="59"/>
     </row>
     <row r="128" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="59"/>
       <c r="B128" s="64" t="s">
+        <v>503</v>
+      </c>
+      <c r="C128" s="64" t="s">
         <v>504</v>
-      </c>
-      <c r="C128" s="64" t="s">
-        <v>505</v>
       </c>
       <c r="D128" s="59"/>
     </row>
     <row r="129" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="59"/>
       <c r="B129" s="65" t="s">
+        <v>505</v>
+      </c>
+      <c r="C129" s="65" t="s">
         <v>506</v>
-      </c>
-      <c r="C129" s="65" t="s">
-        <v>507</v>
       </c>
       <c r="D129" s="59"/>
     </row>
     <row r="130" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="59"/>
       <c r="B130" s="65" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="C130" s="65" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D130" s="59"/>
     </row>
     <row r="131" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="59"/>
       <c r="B131" s="65" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C131" s="65" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="D131" s="59"/>
     </row>
     <row r="132" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="59"/>
       <c r="B132" s="65" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C132" s="65" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D132" s="59"/>
     </row>
     <row r="133" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="59"/>
       <c r="B133" s="65" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C133" s="65" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D133" s="59"/>
     </row>
     <row r="134" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="59"/>
       <c r="B134" s="65" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C134" s="65" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D134" s="59"/>
     </row>
     <row r="135" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="59"/>
       <c r="B135" s="65" t="s">
+        <v>512</v>
+      </c>
+      <c r="C135" s="65" t="s">
         <v>513</v>
-      </c>
-      <c r="C135" s="65" t="s">
-        <v>514</v>
       </c>
       <c r="D135" s="59"/>
     </row>
     <row r="136" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="59"/>
       <c r="B136" s="65" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C136" s="65" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="D136" s="59"/>
     </row>
     <row r="137" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="59"/>
       <c r="B137" s="65" t="s">
+        <v>515</v>
+      </c>
+      <c r="C137" s="65" t="s">
         <v>516</v>
-      </c>
-      <c r="C137" s="65" t="s">
-        <v>517</v>
       </c>
       <c r="D137" s="59"/>
     </row>
     <row r="138" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="59"/>
       <c r="B138" s="65" t="s">
+        <v>517</v>
+      </c>
+      <c r="C138" s="65" t="s">
         <v>518</v>
-      </c>
-      <c r="C138" s="65" t="s">
-        <v>519</v>
       </c>
       <c r="D138" s="59"/>
     </row>
     <row r="139" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="59"/>
       <c r="B139" s="65" t="s">
+        <v>519</v>
+      </c>
+      <c r="C139" s="65" t="s">
         <v>520</v>
-      </c>
-      <c r="C139" s="65" t="s">
-        <v>521</v>
       </c>
       <c r="D139" s="59"/>
     </row>
     <row r="140" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="59"/>
       <c r="B140" s="65" t="s">
+        <v>521</v>
+      </c>
+      <c r="C140" s="65" t="s">
         <v>522</v>
-      </c>
-      <c r="C140" s="65" t="s">
-        <v>523</v>
       </c>
       <c r="D140" s="59"/>
     </row>
     <row r="141" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="59"/>
       <c r="B141" s="65" t="s">
+        <v>523</v>
+      </c>
+      <c r="C141" s="65" t="s">
         <v>524</v>
-      </c>
-      <c r="C141" s="65" t="s">
-        <v>525</v>
       </c>
       <c r="D141" s="59"/>
     </row>
     <row r="142" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="59"/>
       <c r="B142" s="65" t="s">
+        <v>525</v>
+      </c>
+      <c r="C142" s="65" t="s">
         <v>526</v>
-      </c>
-      <c r="C142" s="65" t="s">
-        <v>527</v>
       </c>
       <c r="D142" s="59"/>
     </row>
     <row r="143" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="59"/>
       <c r="B143" s="65" t="s">
+        <v>527</v>
+      </c>
+      <c r="C143" s="65" t="s">
         <v>528</v>
-      </c>
-      <c r="C143" s="65" t="s">
-        <v>529</v>
       </c>
       <c r="D143" s="59"/>
     </row>
     <row r="144" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="59"/>
       <c r="B144" s="65" t="s">
+        <v>529</v>
+      </c>
+      <c r="C144" s="65" t="s">
         <v>530</v>
-      </c>
-      <c r="C144" s="65" t="s">
-        <v>531</v>
       </c>
       <c r="D144" s="59"/>
     </row>
     <row r="145" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="59"/>
       <c r="B145" s="65" t="s">
+        <v>531</v>
+      </c>
+      <c r="C145" s="65" t="s">
         <v>532</v>
-      </c>
-      <c r="C145" s="65" t="s">
-        <v>533</v>
       </c>
       <c r="D145" s="59"/>
     </row>
     <row r="146" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="59"/>
       <c r="B146" s="65" t="s">
+        <v>533</v>
+      </c>
+      <c r="C146" s="65" t="s">
         <v>534</v>
-      </c>
-      <c r="C146" s="65" t="s">
-        <v>535</v>
       </c>
       <c r="D146" s="59"/>
     </row>
     <row r="147" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="59"/>
       <c r="B147" s="65" t="s">
+        <v>535</v>
+      </c>
+      <c r="C147" s="65" t="s">
         <v>536</v>
-      </c>
-      <c r="C147" s="65" t="s">
-        <v>537</v>
       </c>
       <c r="D147" s="59"/>
     </row>
     <row r="148" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="59"/>
       <c r="B148" s="65" t="s">
+        <v>537</v>
+      </c>
+      <c r="C148" s="65" t="s">
         <v>538</v>
-      </c>
-      <c r="C148" s="65" t="s">
-        <v>539</v>
       </c>
       <c r="D148" s="59"/>
     </row>
     <row r="149" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="59"/>
       <c r="B149" s="65" t="s">
+        <v>539</v>
+      </c>
+      <c r="C149" s="65" t="s">
         <v>540</v>
-      </c>
-      <c r="C149" s="65" t="s">
-        <v>541</v>
       </c>
       <c r="D149" s="59"/>
     </row>
     <row r="150" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="59"/>
       <c r="B150" s="65" t="s">
+        <v>541</v>
+      </c>
+      <c r="C150" s="65" t="s">
         <v>542</v>
-      </c>
-      <c r="C150" s="65" t="s">
-        <v>543</v>
       </c>
       <c r="D150" s="59"/>
     </row>
     <row r="151" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="59"/>
       <c r="B151" s="65" t="s">
+        <v>543</v>
+      </c>
+      <c r="C151" s="65" t="s">
         <v>544</v>
-      </c>
-      <c r="C151" s="65" t="s">
-        <v>545</v>
       </c>
       <c r="D151" s="59"/>
     </row>
     <row r="152" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="59"/>
       <c r="B152" s="65" t="s">
+        <v>545</v>
+      </c>
+      <c r="C152" s="65" t="s">
         <v>546</v>
-      </c>
-      <c r="C152" s="65" t="s">
-        <v>547</v>
       </c>
       <c r="D152" s="59"/>
     </row>
     <row r="153" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="59"/>
       <c r="B153" s="65" t="s">
+        <v>547</v>
+      </c>
+      <c r="C153" s="65" t="s">
         <v>548</v>
-      </c>
-      <c r="C153" s="65" t="s">
-        <v>549</v>
       </c>
       <c r="D153" s="59"/>
     </row>
     <row r="154" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="59"/>
       <c r="B154" s="65" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C154" s="65" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="D154" s="59"/>
     </row>
@@ -43752,7 +43746,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="P32:P36 A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -43762,7 +43756,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="43" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B1" s="43"/>
     </row>
@@ -43772,54 +43766,54 @@
     </row>
     <row r="3" customFormat="false" ht="99" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="45" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B3" s="45"/>
     </row>
     <row r="5" s="8" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="B5" s="26" t="s">
         <v>203</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="C5" s="66" t="s">
+        <v>249</v>
+      </c>
+      <c r="D5" s="66" t="s">
+        <v>250</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>357</v>
+      </c>
+      <c r="F5" s="26" t="s">
+        <v>552</v>
+      </c>
+      <c r="G5" s="26" t="s">
         <v>204</v>
-      </c>
-      <c r="C5" s="66" t="s">
-        <v>250</v>
-      </c>
-      <c r="D5" s="66" t="s">
-        <v>251</v>
-      </c>
-      <c r="E5" s="26" t="s">
-        <v>358</v>
-      </c>
-      <c r="F5" s="26" t="s">
-        <v>553</v>
-      </c>
-      <c r="G5" s="26" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="6" s="48" customFormat="true" ht="204.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="47" t="s">
+        <v>553</v>
+      </c>
+      <c r="B6" s="47" t="s">
         <v>554</v>
       </c>
-      <c r="B6" s="47" t="s">
+      <c r="C6" s="47" t="s">
         <v>555</v>
       </c>
-      <c r="C6" s="47" t="s">
+      <c r="D6" s="47" t="s">
+        <v>266</v>
+      </c>
+      <c r="E6" s="47" t="s">
         <v>556</v>
       </c>
-      <c r="D6" s="47" t="s">
-        <v>267</v>
-      </c>
-      <c r="E6" s="47" t="s">
+      <c r="F6" s="47" t="s">
         <v>557</v>
       </c>
-      <c r="F6" s="47" t="s">
+      <c r="G6" s="47" t="s">
         <v>558</v>
-      </c>
-      <c r="G6" s="47" t="s">
-        <v>559</v>
       </c>
       <c r="H6" s="47"/>
     </row>
@@ -43847,7 +43841,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="P32:P36 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -43857,7 +43851,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="67" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B1" s="67"/>
       <c r="C1" s="68"/>
@@ -43875,7 +43869,7 @@
     </row>
     <row r="3" customFormat="false" ht="54.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="45" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B3" s="45"/>
       <c r="C3" s="68"/>
@@ -43893,43 +43887,43 @@
     </row>
     <row r="5" s="4" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="69" t="s">
+        <v>237</v>
+      </c>
+      <c r="B5" s="69" t="s">
         <v>238</v>
       </c>
-      <c r="B5" s="69" t="s">
+      <c r="C5" s="69" t="s">
         <v>239</v>
       </c>
-      <c r="C5" s="69" t="s">
+      <c r="D5" s="69" t="s">
         <v>240</v>
       </c>
-      <c r="D5" s="69" t="s">
+      <c r="E5" s="69" t="s">
+        <v>561</v>
+      </c>
+      <c r="F5" s="70" t="s">
         <v>241</v>
-      </c>
-      <c r="E5" s="69" t="s">
-        <v>562</v>
-      </c>
-      <c r="F5" s="70" t="s">
-        <v>242</v>
       </c>
       <c r="H5" s="7"/>
     </row>
     <row r="6" s="48" customFormat="true" ht="315" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="47" t="s">
+        <v>562</v>
+      </c>
+      <c r="B6" s="47" t="s">
         <v>563</v>
       </c>
-      <c r="B6" s="47" t="s">
+      <c r="C6" s="47" t="s">
         <v>564</v>
       </c>
-      <c r="C6" s="47" t="s">
+      <c r="D6" s="47" t="s">
         <v>565</v>
       </c>
-      <c r="D6" s="47" t="s">
+      <c r="E6" s="47" t="s">
         <v>566</v>
       </c>
-      <c r="E6" s="47" t="s">
+      <c r="F6" s="47" t="s">
         <v>567</v>
-      </c>
-      <c r="F6" s="47" t="s">
-        <v>568</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>